<commit_message>
Implemented more logic for cohort in backend, changed AddRowStrategy to use decorator, wrote more test case
</commit_message>
<xml_diff>
--- a/tests/testMaterials/CDS_SPARSE_2013_2014.xlsx
+++ b/tests/testMaterials/CDS_SPARSE_2013_2014.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\CDSData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\tests\testMaterials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A4229F-B632-455F-B4CA-17C012180D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723D1CD6-619D-45A6-BB85-E01C92012552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -401,8 +401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -640,7 +640,7 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>